<commit_message>
ajout du move de l'xlsx à la derniere iteration
</commit_message>
<xml_diff>
--- a/015251/TS_Themis VASILIKIOTIS.xlsx
+++ b/015251/TS_Themis VASILIKIOTIS.xlsx
@@ -14,7 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <x:si>
+    <x:t>JULY 2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20,0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AUGUST 2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14.0</x:t>
+  </x:si>
   <x:si>
     <x:t>SEPTEMBER 2024</x:t>
   </x:si>
@@ -384,6 +396,22 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>